<commit_message>
Atualização de horas trabalhadas no desenvolvimento
</commit_message>
<xml_diff>
--- a/018 - Grafico BurnDown.xlsx
+++ b/018 - Grafico BurnDown.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttava\OneDrive\Documents\Engenharia de Computação\8ºPERIODO\PRATICA EM FABRICA DE SOFTWARE I\Fabrica-de-Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="16" documentId="C5AE2610A17A9795ABCE8FE03CED8E3DAB10E969" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{9E938DBE-C0C6-45EF-9848-8D9ECCD93619}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="7770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grafico" sheetId="2" r:id="rId1"/>
     <sheet name="Dados" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -177,7 +178,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,15 +347,6 @@
     <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -366,6 +358,15 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,7 +432,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -499,124 +499,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>21</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>21</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>21</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>21</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -853,7 +853,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -975,7 +974,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1048,7 +1046,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1675,7 +1672,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1955,7 +1958,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1973,11 +1976,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AQ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21:W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,13 +2124,13 @@
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="13">
         <v>5</v>
       </c>
       <c r="D2" s="4"/>
@@ -2147,7 +2150,9 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
+      <c r="U2" s="4">
+        <v>2</v>
+      </c>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
@@ -2167,21 +2172,21 @@
       <c r="AL2" s="4"/>
       <c r="AM2" s="4"/>
       <c r="AN2" s="4"/>
-      <c r="AO2" s="4"/>
+      <c r="AO2" s="4">
+        <v>3</v>
+      </c>
       <c r="AP2" s="4"/>
       <c r="AQ2" s="4"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="13">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -2199,7 +2204,9 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
+      <c r="V3" s="4">
+        <v>4</v>
+      </c>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
@@ -2219,15 +2226,17 @@
       <c r="AM3" s="4"/>
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
-      <c r="AP3" s="4"/>
+      <c r="AP3" s="4">
+        <v>4</v>
+      </c>
       <c r="AQ3" s="4"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="13">
         <v>10</v>
       </c>
       <c r="D4" s="4"/>
@@ -2238,9 +2247,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="4">
-        <v>1</v>
-      </c>
+      <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -2251,7 +2258,9 @@
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
+      <c r="W4" s="4">
+        <v>5</v>
+      </c>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
@@ -2272,130 +2281,130 @@
       <c r="AO4" s="4"/>
       <c r="AP4" s="4"/>
       <c r="AQ4" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="12"/>
-      <c r="AI5" s="12"/>
-      <c r="AJ5" s="12"/>
-      <c r="AK5" s="12"/>
-      <c r="AL5" s="12"/>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
-      <c r="AO5" s="12"/>
-      <c r="AP5" s="12"/>
-      <c r="AQ5" s="13"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="16"/>
+      <c r="AJ5" s="16"/>
+      <c r="AK5" s="16"/>
+      <c r="AL5" s="16"/>
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="16"/>
+      <c r="AP5" s="16"/>
+      <c r="AQ5" s="17"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <f>SUM(C2:C4)</f>
         <v>23</v>
       </c>
       <c r="D6" s="7">
         <f>C6-SUM(D2:D5)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" ref="E6:F6" si="0">D6-SUM(E2:E5)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7">
         <f t="shared" ref="G6" si="1">F6-SUM(G2:G5)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H6" s="7">
         <f t="shared" ref="H6" si="2">G6-SUM(H2:H5)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" ref="I6" si="3">H6-SUM(I2:I5)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J6" s="7">
         <f t="shared" ref="J6" si="4">I6-SUM(J2:J5)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" ref="K6" si="5">J6-SUM(K2:K5)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L6" s="7">
         <f t="shared" ref="L6" si="6">K6-SUM(L2:L5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M6" s="7">
         <f t="shared" ref="M6" si="7">L6-SUM(M2:M5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" ref="N6" si="8">M6-SUM(N2:N5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O6" s="7">
         <f t="shared" ref="O6" si="9">N6-SUM(O2:O5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P6" s="7">
         <f t="shared" ref="P6" si="10">O6-SUM(P2:P5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q6" s="7">
         <f t="shared" ref="Q6" si="11">P6-SUM(Q2:Q5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R6" s="7">
         <f t="shared" ref="R6" si="12">Q6-SUM(R2:R5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="S6" s="7">
         <f t="shared" ref="S6" si="13">R6-SUM(S2:S5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="T6" s="7">
         <f t="shared" ref="T6" si="14">S6-SUM(T2:T5)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="U6" s="7">
         <f t="shared" ref="U6" si="15">T6-SUM(U2:U5)</f>
@@ -2403,99 +2412,99 @@
       </c>
       <c r="V6" s="7">
         <f t="shared" ref="V6" si="16">U6-SUM(V2:V5)</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="W6" s="7">
         <f t="shared" ref="W6" si="17">V6-SUM(W2:W5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="X6" s="7">
         <f t="shared" ref="X6" si="18">W6-SUM(X2:X5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="Y6" s="7">
         <f t="shared" ref="Y6" si="19">X6-SUM(Y2:Y5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="Z6" s="7">
         <f t="shared" ref="Z6" si="20">Y6-SUM(Z2:Z5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AA6" s="7">
         <f t="shared" ref="AA6" si="21">Z6-SUM(AA2:AA5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AB6" s="7">
         <f t="shared" ref="AB6" si="22">AA6-SUM(AB2:AB5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AC6" s="7">
         <f t="shared" ref="AC6" si="23">AB6-SUM(AC2:AC5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AD6" s="7">
         <f t="shared" ref="AD6" si="24">AC6-SUM(AD2:AD5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AE6" s="7">
         <f t="shared" ref="AE6" si="25">AD6-SUM(AE2:AE5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AF6" s="7">
         <f t="shared" ref="AF6" si="26">AE6-SUM(AF2:AF5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AG6" s="7">
         <f t="shared" ref="AG6" si="27">AF6-SUM(AG2:AG5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AH6" s="7">
         <f t="shared" ref="AH6" si="28">AG6-SUM(AH2:AH5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AI6" s="7">
         <f t="shared" ref="AI6" si="29">AH6-SUM(AI2:AI5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AJ6" s="7">
         <f t="shared" ref="AJ6" si="30">AI6-SUM(AJ2:AJ5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AK6" s="7">
         <f t="shared" ref="AK6" si="31">AJ6-SUM(AK2:AK5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AL6" s="7">
         <f t="shared" ref="AL6" si="32">AK6-SUM(AL2:AL5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AM6" s="7">
         <f t="shared" ref="AM6" si="33">AL6-SUM(AM2:AM5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AN6" s="7">
         <f t="shared" ref="AN6" si="34">AM6-SUM(AN2:AN5)</f>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="AO6" s="7">
-        <f t="shared" ref="AO6" si="35">AN6-SUM(AO2:AO5)</f>
-        <v>21</v>
+        <f>AN6-SUM(AO2:AO5)</f>
+        <v>9</v>
       </c>
       <c r="AP6" s="7">
-        <f t="shared" ref="AP6" si="36">AO6-SUM(AP2:AP5)</f>
-        <v>21</v>
+        <f t="shared" ref="AP6" si="35">AO6-SUM(AP2:AP5)</f>
+        <v>5</v>
       </c>
       <c r="AQ6" s="7">
-        <f t="shared" ref="AQ6" si="37">AP6-SUM(AQ2:AQ5)</f>
-        <v>19</v>
+        <f>AP6-SUM(AQ2:AQ5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <f>SUM(C2:C4)</f>
         <v>23</v>
       </c>
@@ -2504,159 +2513,159 @@
         <v>22.425000000000001</v>
       </c>
       <c r="E7" s="9">
-        <f t="shared" ref="E7:AQ7" si="38">D7-($C$7/COUNTA($D$1:$AQ$1))</f>
+        <f t="shared" ref="E7:AQ7" si="36">D7-($C$7/COUNTA($D$1:$AQ$1))</f>
         <v>21.85</v>
       </c>
       <c r="F7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>21.275000000000002</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>20.700000000000003</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>20.125000000000004</v>
       </c>
       <c r="I7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>19.550000000000004</v>
       </c>
       <c r="J7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>18.975000000000005</v>
       </c>
       <c r="K7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>18.400000000000006</v>
       </c>
       <c r="L7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>17.825000000000006</v>
       </c>
       <c r="M7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>17.250000000000007</v>
       </c>
       <c r="N7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>16.675000000000008</v>
       </c>
       <c r="O7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>16.100000000000009</v>
       </c>
       <c r="P7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>15.525000000000009</v>
       </c>
       <c r="Q7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>14.95000000000001</v>
       </c>
       <c r="R7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>14.375000000000011</v>
       </c>
       <c r="S7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>13.800000000000011</v>
       </c>
       <c r="T7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>13.225000000000012</v>
       </c>
       <c r="U7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>12.650000000000013</v>
       </c>
       <c r="V7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>12.075000000000014</v>
       </c>
       <c r="W7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>11.500000000000014</v>
       </c>
       <c r="X7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>10.925000000000015</v>
       </c>
       <c r="Y7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>10.350000000000016</v>
       </c>
       <c r="Z7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>9.7750000000000163</v>
       </c>
       <c r="AA7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>9.2000000000000171</v>
       </c>
       <c r="AB7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>8.6250000000000178</v>
       </c>
       <c r="AC7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>8.0500000000000185</v>
       </c>
       <c r="AD7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>7.4750000000000183</v>
       </c>
       <c r="AE7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>6.9000000000000181</v>
       </c>
       <c r="AF7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>6.3250000000000179</v>
       </c>
       <c r="AG7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>5.7500000000000178</v>
       </c>
       <c r="AH7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>5.1750000000000176</v>
       </c>
       <c r="AI7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>4.6000000000000174</v>
       </c>
       <c r="AJ7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>4.0250000000000172</v>
       </c>
       <c r="AK7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>3.4500000000000171</v>
       </c>
       <c r="AL7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>2.8750000000000169</v>
       </c>
       <c r="AM7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>2.3000000000000167</v>
       </c>
       <c r="AN7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>1.7250000000000167</v>
       </c>
       <c r="AO7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>1.1500000000000168</v>
       </c>
       <c r="AP7" s="9">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>0.57500000000001683</v>
       </c>
       <c r="AQ7" s="10">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>1.6875389974302379E-14</v>
       </c>
     </row>

</xml_diff>